<commit_message>
Changed to closed loop belt
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simon\Documents\GitHub\Brailleprinter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{860C0722-15FF-482A-B110-46978E7A7F16}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B4857EA-9445-45B4-81F0-113CACC6EDA5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="10416" windowHeight="4224" xr2:uid="{110836C7-179D-4ECB-89DE-92B610AE0A25}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="261">
   <si>
     <t>Bill of Materials</t>
   </si>
@@ -565,15 +565,9 @@
     <t>Closed loop 2GT belt</t>
   </si>
   <si>
-    <t>2GT belt</t>
-  </si>
-  <si>
     <t>188mm x 6mm</t>
   </si>
   <si>
-    <t>525mm x 6mm</t>
-  </si>
-  <si>
     <t>94T / 188mm</t>
   </si>
   <si>
@@ -841,9 +835,6 @@
     <t>https://www.aliexpress.com/item/1005002575803340.html</t>
   </si>
   <si>
-    <t>https://www.aliexpress.com/item/32918948939.html</t>
-  </si>
-  <si>
     <t>https://www.aliexpress.com/item/1005003068711960.html</t>
   </si>
   <si>
@@ -863,6 +854,12 @@
   </si>
   <si>
     <t>617</t>
+  </si>
+  <si>
+    <t>242mm x 6mm</t>
+  </si>
+  <si>
+    <t>https://www.aliexpress.com/item/1005003269480958.html</t>
   </si>
 </sst>
 </file>
@@ -1327,8 +1324,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78217E55-B613-4EDB-95A0-F9D70FDA8662}">
   <dimension ref="A1:H87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="D79" sqref="D79"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1443,7 +1440,7 @@
         <v>12</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>15</v>
@@ -1455,13 +1452,13 @@
         <v>1</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="G7" s="11">
         <v>11.78</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
@@ -1706,7 +1703,7 @@
         <v>2</v>
       </c>
       <c r="F20" s="12" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="G20" s="14">
         <v>24</v>
@@ -1730,7 +1727,7 @@
         <v>1</v>
       </c>
       <c r="F21" s="12" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="G21" s="14">
         <v>1.1399999999999999</v>
@@ -1754,7 +1751,7 @@
         <v>1</v>
       </c>
       <c r="F22" s="12" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="G22" s="14">
         <v>0.7</v>
@@ -1778,7 +1775,7 @@
         <v>2</v>
       </c>
       <c r="F23" s="12" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="G23" s="14">
         <v>0.82</v>
@@ -1802,7 +1799,7 @@
         <v>1</v>
       </c>
       <c r="F24" s="12" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="G24" s="14">
         <v>0.82</v>
@@ -1814,10 +1811,10 @@
         <v>147</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>164</v>
+        <v>259</v>
       </c>
       <c r="D25" s="12" t="s">
         <v>28</v>
@@ -1826,10 +1823,10 @@
         <v>1</v>
       </c>
       <c r="F25" s="12" t="s">
-        <v>254</v>
+        <v>260</v>
       </c>
       <c r="G25" s="14">
-        <v>0.83</v>
+        <v>1.08</v>
       </c>
       <c r="H25" s="12"/>
     </row>
@@ -1841,7 +1838,7 @@
         <v>161</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D26" s="12" t="s">
         <v>28</v>
@@ -1850,13 +1847,13 @@
         <v>1</v>
       </c>
       <c r="F26" s="12" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="G26" s="14">
         <v>1.59</v>
       </c>
       <c r="H26" s="12" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
@@ -1966,7 +1963,7 @@
         <v>1</v>
       </c>
       <c r="F32" s="12" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="G32" s="14">
         <v>1.94</v>
@@ -2029,7 +2026,7 @@
         <v>146</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D35" s="12" t="s">
         <v>143</v>
@@ -2038,7 +2035,7 @@
         <v>10</v>
       </c>
       <c r="F35" s="12" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="G35" s="14">
         <v>1.38</v>
@@ -2050,7 +2047,7 @@
         <v>158</v>
       </c>
       <c r="B36" s="12" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="C36" s="12" t="s">
         <v>159</v>
@@ -2071,13 +2068,13 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" s="12" t="s">
+        <v>207</v>
+      </c>
+      <c r="B37" s="12" t="s">
+        <v>208</v>
+      </c>
+      <c r="C37" s="12" t="s">
         <v>209</v>
-      </c>
-      <c r="B37" s="12" t="s">
-        <v>210</v>
-      </c>
-      <c r="C37" s="12" t="s">
-        <v>211</v>
       </c>
       <c r="D37" s="12" t="s">
         <v>19</v>
@@ -2095,7 +2092,7 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" s="19" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B39" s="19"/>
       <c r="C39" s="19"/>
@@ -2107,13 +2104,13 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" s="9" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B40" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="C40" s="3" t="s">
         <v>166</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>168</v>
       </c>
       <c r="D40" s="3" t="s">
         <v>19</v>
@@ -2130,13 +2127,13 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="B41" s="12" t="s">
+        <v>168</v>
+      </c>
+      <c r="C41" s="3" t="s">
         <v>169</v>
-      </c>
-      <c r="B41" s="12" t="s">
-        <v>170</v>
-      </c>
-      <c r="C41" s="3" t="s">
-        <v>171</v>
       </c>
       <c r="D41" s="3" t="s">
         <v>19</v>
@@ -2153,13 +2150,13 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="B42" s="12" t="s">
+        <v>171</v>
+      </c>
+      <c r="C42" s="3" t="s">
         <v>172</v>
-      </c>
-      <c r="B42" s="12" t="s">
-        <v>173</v>
-      </c>
-      <c r="C42" s="3" t="s">
-        <v>174</v>
       </c>
       <c r="D42" s="3" t="s">
         <v>28</v>
@@ -2168,7 +2165,7 @@
         <v>6</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="G42" s="11">
         <v>17.2</v>
@@ -2176,13 +2173,13 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43" s="9" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B43" s="12" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D43" s="3" t="s">
         <v>19</v>
@@ -2194,21 +2191,21 @@
         <v>11</v>
       </c>
       <c r="H43" s="3" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" s="9" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B44" s="12" t="s">
+        <v>176</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="D44" s="3" t="s">
         <v>178</v>
-      </c>
-      <c r="C44" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="D44" s="3" t="s">
-        <v>180</v>
       </c>
       <c r="E44" s="10">
         <v>1</v>
@@ -2220,21 +2217,21 @@
         <v>0</v>
       </c>
       <c r="H44" s="3" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45" s="9" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B45" s="12" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E45" s="10">
         <v>1</v>
@@ -2244,18 +2241,18 @@
       </c>
       <c r="G45" s="20"/>
       <c r="H45" s="3" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46" s="9" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B46" s="12" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D46" s="3" t="s">
         <v>13</v>
@@ -2264,7 +2261,7 @@
         <v>6</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="G46" s="11">
         <v>5.51</v>
@@ -2272,16 +2269,16 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47" s="9" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B47" s="12" t="s">
+        <v>188</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="D47" s="3" t="s">
         <v>190</v>
-      </c>
-      <c r="C47" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="D47" s="3" t="s">
-        <v>192</v>
       </c>
       <c r="E47" s="10">
         <v>1</v>
@@ -2295,13 +2292,13 @@
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="B48" s="12" t="s">
+        <v>195</v>
+      </c>
+      <c r="C48" s="3" t="s">
         <v>196</v>
-      </c>
-      <c r="B48" s="12" t="s">
-        <v>197</v>
-      </c>
-      <c r="C48" s="3" t="s">
-        <v>198</v>
       </c>
       <c r="D48" s="3" t="s">
         <v>28</v>
@@ -2313,18 +2310,18 @@
         <v>11</v>
       </c>
       <c r="H48" s="3" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="B49" s="12" t="s">
+        <v>200</v>
+      </c>
+      <c r="C49" s="3" t="s">
         <v>201</v>
-      </c>
-      <c r="B49" s="12" t="s">
-        <v>202</v>
-      </c>
-      <c r="C49" s="3" t="s">
-        <v>203</v>
       </c>
       <c r="D49" s="3" t="s">
         <v>28</v>
@@ -2333,13 +2330,13 @@
         <v>1</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="G49" s="11">
         <v>1.3</v>
       </c>
       <c r="H49" s="3" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.3">
@@ -2359,7 +2356,7 @@
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A53" s="15" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B53" s="12" t="s">
         <v>99</v>
@@ -2385,7 +2382,7 @@
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54" s="9" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B54" s="3" t="s">
         <v>26</v>
@@ -2411,7 +2408,7 @@
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55" s="15" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B55" s="3" t="s">
         <v>95</v>
@@ -2437,7 +2434,7 @@
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A56" s="9" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B56" s="3" t="s">
         <v>64</v>
@@ -2460,7 +2457,7 @@
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A57" s="15" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B57" s="3" t="s">
         <v>62</v>
@@ -2483,7 +2480,7 @@
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58" s="9" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B58" s="3" t="s">
         <v>69</v>
@@ -2509,7 +2506,7 @@
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A59" s="15" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B59" s="3" t="s">
         <v>73</v>
@@ -2532,7 +2529,7 @@
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A60" s="9" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B60" s="3" t="s">
         <v>75</v>
@@ -2558,7 +2555,7 @@
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A61" s="15" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B61" s="3" t="s">
         <v>79</v>
@@ -2578,7 +2575,7 @@
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A62" s="9" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B62" s="3" t="s">
         <v>82</v>
@@ -2604,7 +2601,7 @@
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A63" s="15" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B63" s="3" t="s">
         <v>85</v>
@@ -2630,7 +2627,7 @@
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A64" s="9" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B64" s="3" t="s">
         <v>88</v>
@@ -2654,7 +2651,7 @@
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A65" s="15" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B65" s="3" t="s">
         <v>89</v>
@@ -2680,7 +2677,7 @@
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A66" s="9" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B66" s="3" t="s">
         <v>92</v>
@@ -2703,7 +2700,7 @@
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A67" s="15" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B67" s="3" t="s">
         <v>112</v>
@@ -2729,13 +2726,13 @@
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A68" s="9" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C68" s="9" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D68" s="3" t="s">
         <v>28</v>
@@ -2762,10 +2759,10 @@
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A71" s="9" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C71" s="3" t="s">
         <v>120</v>
@@ -2785,10 +2782,10 @@
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A72" s="9" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C72" s="3" t="s">
         <v>36</v>
@@ -2806,10 +2803,10 @@
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A73" s="9" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C73" s="3" t="s">
         <v>33</v>
@@ -2827,10 +2824,10 @@
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A74" s="9" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C74" s="3" t="s">
         <v>118</v>
@@ -2848,13 +2845,13 @@
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A75" s="9" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D75" s="3" t="s">
         <v>13</v>
@@ -2869,10 +2866,10 @@
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A76" s="9" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C76" s="3" t="s">
         <v>110</v>
@@ -2890,10 +2887,10 @@
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A77" s="9" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C77" s="3" t="s">
         <v>109</v>
@@ -2911,10 +2908,10 @@
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A78" s="9" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C78" s="3" t="s">
         <v>108</v>
@@ -2932,10 +2929,10 @@
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A79" s="9" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C79" s="3" t="s">
         <v>107</v>
@@ -2956,10 +2953,10 @@
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A80" s="9" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C80" s="3" t="s">
         <v>36</v>
@@ -2977,10 +2974,10 @@
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A81" s="9" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C81" s="3" t="s">
         <v>157</v>
@@ -2998,10 +2995,10 @@
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A82" s="9" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C82" s="3" t="s">
         <v>33</v>
@@ -3019,10 +3016,10 @@
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A83" s="9" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C83" s="3" t="s">
         <v>118</v>
@@ -3040,13 +3037,13 @@
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A84" s="9" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D84" s="3" t="s">
         <v>13</v>
@@ -3061,16 +3058,16 @@
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A85" s="9" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C85" s="3" t="s">
         <v>123</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="E85" s="10">
         <v>2</v>
@@ -3082,7 +3079,7 @@
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A86" s="9" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B86" s="3" t="s">
         <v>121</v>
@@ -3106,7 +3103,7 @@
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A87" s="9" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="B87" s="3" t="s">
         <v>121</v>
@@ -3222,7 +3219,7 @@
         <v>32</v>
       </c>
       <c r="B4" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C4" t="s">
         <v>13</v>
@@ -3384,7 +3381,7 @@
         <v>32</v>
       </c>
       <c r="B13" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C13" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
Optimized paper feed mechanism
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20387"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20389"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simon\Documents\GitHub\Brailleprinter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B4857EA-9445-45B4-81F0-113CACC6EDA5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B042A8B-9094-4208-B229-28D493C99CEC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="10416" windowHeight="4224" xr2:uid="{110836C7-179D-4ECB-89DE-92B610AE0A25}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="262">
   <si>
     <t>Bill of Materials</t>
   </si>
@@ -565,12 +565,6 @@
     <t>Closed loop 2GT belt</t>
   </si>
   <si>
-    <t>188mm x 6mm</t>
-  </si>
-  <si>
-    <t>94T / 188mm</t>
-  </si>
-  <si>
     <t>Carriage</t>
   </si>
   <si>
@@ -856,10 +850,19 @@
     <t>617</t>
   </si>
   <si>
-    <t>242mm x 6mm</t>
-  </si>
-  <si>
-    <t>https://www.aliexpress.com/item/1005003269480958.html</t>
+    <t>200mm x 6mm</t>
+  </si>
+  <si>
+    <t>524mm x 6mm</t>
+  </si>
+  <si>
+    <t>100T / 200mm</t>
+  </si>
+  <si>
+    <t>262T / 564mm</t>
+  </si>
+  <si>
+    <t>https://www.aliexpress.com/item/1005004107020953.html</t>
   </si>
 </sst>
 </file>
@@ -944,7 +947,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1007,6 +1010,7 @@
     <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -1324,8 +1328,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78217E55-B613-4EDB-95A0-F9D70FDA8662}">
   <dimension ref="A1:H87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1440,7 +1444,7 @@
         <v>12</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>15</v>
@@ -1452,13 +1456,13 @@
         <v>1</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="G7" s="11">
         <v>11.78</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
@@ -1703,7 +1707,7 @@
         <v>2</v>
       </c>
       <c r="F20" s="12" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="G20" s="14">
         <v>24</v>
@@ -1727,7 +1731,7 @@
         <v>1</v>
       </c>
       <c r="F21" s="12" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="G21" s="14">
         <v>1.1399999999999999</v>
@@ -1751,7 +1755,7 @@
         <v>1</v>
       </c>
       <c r="F22" s="12" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="G22" s="14">
         <v>0.7</v>
@@ -1775,7 +1779,7 @@
         <v>2</v>
       </c>
       <c r="F23" s="12" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="G23" s="14">
         <v>0.82</v>
@@ -1799,7 +1803,7 @@
         <v>1</v>
       </c>
       <c r="F24" s="12" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="G24" s="14">
         <v>0.82</v>
@@ -1814,7 +1818,7 @@
         <v>161</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D25" s="12" t="s">
         <v>28</v>
@@ -1823,12 +1827,14 @@
         <v>1</v>
       </c>
       <c r="F25" s="12" t="s">
+        <v>261</v>
+      </c>
+      <c r="G25" s="14">
+        <v>2.23</v>
+      </c>
+      <c r="H25" s="12" t="s">
         <v>260</v>
       </c>
-      <c r="G25" s="14">
-        <v>1.08</v>
-      </c>
-      <c r="H25" s="12"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="12" t="s">
@@ -1838,7 +1844,7 @@
         <v>161</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>162</v>
+        <v>257</v>
       </c>
       <c r="D26" s="12" t="s">
         <v>28</v>
@@ -1846,14 +1852,14 @@
       <c r="E26" s="13">
         <v>1</v>
       </c>
-      <c r="F26" s="12" t="s">
-        <v>251</v>
+      <c r="F26" s="22" t="s">
+        <v>249</v>
       </c>
       <c r="G26" s="14">
-        <v>1.59</v>
+        <v>1.64</v>
       </c>
       <c r="H26" s="12" t="s">
-        <v>163</v>
+        <v>259</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
@@ -1963,7 +1969,7 @@
         <v>1</v>
       </c>
       <c r="F32" s="12" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="G32" s="14">
         <v>1.94</v>
@@ -2026,7 +2032,7 @@
         <v>146</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D35" s="12" t="s">
         <v>143</v>
@@ -2035,7 +2041,7 @@
         <v>10</v>
       </c>
       <c r="F35" s="12" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="G35" s="14">
         <v>1.38</v>
@@ -2047,7 +2053,7 @@
         <v>158</v>
       </c>
       <c r="B36" s="12" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C36" s="12" t="s">
         <v>159</v>
@@ -2068,13 +2074,13 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" s="12" t="s">
+        <v>205</v>
+      </c>
+      <c r="B37" s="12" t="s">
+        <v>206</v>
+      </c>
+      <c r="C37" s="12" t="s">
         <v>207</v>
-      </c>
-      <c r="B37" s="12" t="s">
-        <v>208</v>
-      </c>
-      <c r="C37" s="12" t="s">
-        <v>209</v>
       </c>
       <c r="D37" s="12" t="s">
         <v>19</v>
@@ -2092,7 +2098,7 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" s="19" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B39" s="19"/>
       <c r="C39" s="19"/>
@@ -2104,13 +2110,13 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" s="9" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B40" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="C40" s="3" t="s">
         <v>164</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>166</v>
       </c>
       <c r="D40" s="3" t="s">
         <v>19</v>
@@ -2127,13 +2133,13 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="B41" s="12" t="s">
+        <v>166</v>
+      </c>
+      <c r="C41" s="3" t="s">
         <v>167</v>
-      </c>
-      <c r="B41" s="12" t="s">
-        <v>168</v>
-      </c>
-      <c r="C41" s="3" t="s">
-        <v>169</v>
       </c>
       <c r="D41" s="3" t="s">
         <v>19</v>
@@ -2150,13 +2156,13 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="B42" s="12" t="s">
+        <v>169</v>
+      </c>
+      <c r="C42" s="3" t="s">
         <v>170</v>
-      </c>
-      <c r="B42" s="12" t="s">
-        <v>171</v>
-      </c>
-      <c r="C42" s="3" t="s">
-        <v>172</v>
       </c>
       <c r="D42" s="3" t="s">
         <v>28</v>
@@ -2165,7 +2171,7 @@
         <v>6</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="G42" s="11">
         <v>17.2</v>
@@ -2173,13 +2179,13 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43" s="9" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B43" s="12" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D43" s="3" t="s">
         <v>19</v>
@@ -2191,21 +2197,21 @@
         <v>11</v>
       </c>
       <c r="H43" s="3" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" s="9" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B44" s="12" t="s">
+        <v>174</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="D44" s="3" t="s">
         <v>176</v>
-      </c>
-      <c r="C44" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="D44" s="3" t="s">
-        <v>178</v>
       </c>
       <c r="E44" s="10">
         <v>1</v>
@@ -2217,21 +2223,21 @@
         <v>0</v>
       </c>
       <c r="H44" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45" s="9" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B45" s="12" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E45" s="10">
         <v>1</v>
@@ -2241,18 +2247,18 @@
       </c>
       <c r="G45" s="20"/>
       <c r="H45" s="3" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46" s="9" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B46" s="12" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D46" s="3" t="s">
         <v>13</v>
@@ -2261,7 +2267,7 @@
         <v>6</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="G46" s="11">
         <v>5.51</v>
@@ -2269,16 +2275,16 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47" s="9" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B47" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="D47" s="3" t="s">
         <v>188</v>
-      </c>
-      <c r="C47" s="3" t="s">
-        <v>189</v>
-      </c>
-      <c r="D47" s="3" t="s">
-        <v>190</v>
       </c>
       <c r="E47" s="10">
         <v>1</v>
@@ -2292,13 +2298,13 @@
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48" s="9" t="s">
+        <v>192</v>
+      </c>
+      <c r="B48" s="12" t="s">
+        <v>193</v>
+      </c>
+      <c r="C48" s="3" t="s">
         <v>194</v>
-      </c>
-      <c r="B48" s="12" t="s">
-        <v>195</v>
-      </c>
-      <c r="C48" s="3" t="s">
-        <v>196</v>
       </c>
       <c r="D48" s="3" t="s">
         <v>28</v>
@@ -2310,18 +2316,18 @@
         <v>11</v>
       </c>
       <c r="H48" s="3" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49" s="9" t="s">
+        <v>197</v>
+      </c>
+      <c r="B49" s="12" t="s">
+        <v>198</v>
+      </c>
+      <c r="C49" s="3" t="s">
         <v>199</v>
-      </c>
-      <c r="B49" s="12" t="s">
-        <v>200</v>
-      </c>
-      <c r="C49" s="3" t="s">
-        <v>201</v>
       </c>
       <c r="D49" s="3" t="s">
         <v>28</v>
@@ -2330,13 +2336,13 @@
         <v>1</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="G49" s="11">
         <v>1.3</v>
       </c>
       <c r="H49" s="3" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.3">
@@ -2356,7 +2362,7 @@
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A53" s="15" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B53" s="12" t="s">
         <v>99</v>
@@ -2382,7 +2388,7 @@
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54" s="9" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B54" s="3" t="s">
         <v>26</v>
@@ -2408,7 +2414,7 @@
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55" s="15" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B55" s="3" t="s">
         <v>95</v>
@@ -2434,7 +2440,7 @@
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A56" s="9" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B56" s="3" t="s">
         <v>64</v>
@@ -2457,7 +2463,7 @@
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A57" s="15" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B57" s="3" t="s">
         <v>62</v>
@@ -2480,7 +2486,7 @@
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58" s="9" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B58" s="3" t="s">
         <v>69</v>
@@ -2506,7 +2512,7 @@
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A59" s="15" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B59" s="3" t="s">
         <v>73</v>
@@ -2529,7 +2535,7 @@
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A60" s="9" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B60" s="3" t="s">
         <v>75</v>
@@ -2555,7 +2561,7 @@
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A61" s="15" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B61" s="3" t="s">
         <v>79</v>
@@ -2575,7 +2581,7 @@
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A62" s="9" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B62" s="3" t="s">
         <v>82</v>
@@ -2601,7 +2607,7 @@
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A63" s="15" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B63" s="3" t="s">
         <v>85</v>
@@ -2627,7 +2633,7 @@
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A64" s="9" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B64" s="3" t="s">
         <v>88</v>
@@ -2651,7 +2657,7 @@
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A65" s="15" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B65" s="3" t="s">
         <v>89</v>
@@ -2677,7 +2683,7 @@
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A66" s="9" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B66" s="3" t="s">
         <v>92</v>
@@ -2700,7 +2706,7 @@
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A67" s="15" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B67" s="3" t="s">
         <v>112</v>
@@ -2726,13 +2732,13 @@
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A68" s="9" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C68" s="9" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D68" s="3" t="s">
         <v>28</v>
@@ -2759,10 +2765,10 @@
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A71" s="9" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C71" s="3" t="s">
         <v>120</v>
@@ -2782,10 +2788,10 @@
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A72" s="9" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C72" s="3" t="s">
         <v>36</v>
@@ -2803,10 +2809,10 @@
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A73" s="9" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C73" s="3" t="s">
         <v>33</v>
@@ -2824,10 +2830,10 @@
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A74" s="9" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C74" s="3" t="s">
         <v>118</v>
@@ -2845,13 +2851,13 @@
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A75" s="9" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D75" s="3" t="s">
         <v>13</v>
@@ -2866,10 +2872,10 @@
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A76" s="9" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C76" s="3" t="s">
         <v>110</v>
@@ -2887,10 +2893,10 @@
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A77" s="9" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C77" s="3" t="s">
         <v>109</v>
@@ -2908,10 +2914,10 @@
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A78" s="9" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C78" s="3" t="s">
         <v>108</v>
@@ -2929,10 +2935,10 @@
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A79" s="9" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C79" s="3" t="s">
         <v>107</v>
@@ -2953,10 +2959,10 @@
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A80" s="9" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C80" s="3" t="s">
         <v>36</v>
@@ -2974,10 +2980,10 @@
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A81" s="9" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C81" s="3" t="s">
         <v>157</v>
@@ -2995,10 +3001,10 @@
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A82" s="9" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C82" s="3" t="s">
         <v>33</v>
@@ -3016,10 +3022,10 @@
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A83" s="9" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C83" s="3" t="s">
         <v>118</v>
@@ -3037,13 +3043,13 @@
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A84" s="9" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D84" s="3" t="s">
         <v>13</v>
@@ -3058,16 +3064,16 @@
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A85" s="9" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C85" s="3" t="s">
         <v>123</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="E85" s="10">
         <v>2</v>
@@ -3079,7 +3085,7 @@
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A86" s="9" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B86" s="3" t="s">
         <v>121</v>
@@ -3103,7 +3109,7 @@
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A87" s="9" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B87" s="3" t="s">
         <v>121</v>
@@ -3219,7 +3225,7 @@
         <v>32</v>
       </c>
       <c r="B4" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="C4" t="s">
         <v>13</v>
@@ -3381,7 +3387,7 @@
         <v>32</v>
       </c>
       <c r="B13" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C13" t="s">
         <v>13</v>

</xml_diff>